<commit_message>
Model with Dynamic Yearly Volume Calculations
Added rules to calculate EWA, Project Supply, & etc. These take into consideration the observed flows. In addition, the dilution ramp rates and triggers are now calculated within the model. Temporary RiverWise file has been created for review.
</commit_message>
<xml_diff>
--- a/Database/Ingest/flowcalc.xlsx
+++ b/Database/Ingest/flowcalc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Models\Mitch\KlamathOpsModel\DMI Sheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Models\Mitch\KlamathOpsModel\Database\Ingest\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -6239,7 +6239,7 @@
         </row>
         <row r="1160">
           <cell r="C1160">
-            <v>287.60330578512395</v>
+            <v>297.52066115702479</v>
           </cell>
           <cell r="AQ1160">
             <v>0</v>
@@ -6294,7 +6294,7 @@
         </row>
         <row r="1165">
           <cell r="C1165">
-            <v>156.099173553719</v>
+            <v>297.52066115702479</v>
           </cell>
           <cell r="AQ1165">
             <v>0</v>
@@ -6305,7 +6305,7 @@
         </row>
         <row r="1166">
           <cell r="C1166">
-            <v>162.04958677685951</v>
+            <v>297.52066115702479</v>
           </cell>
           <cell r="AQ1166">
             <v>0</v>
@@ -6327,7 +6327,7 @@
         </row>
         <row r="1168">
           <cell r="C1168">
-            <v>200.3305785123967</v>
+            <v>297.52066115702479</v>
           </cell>
           <cell r="AQ1168">
             <v>0</v>
@@ -9356,8 +9356,8 @@
   <dimension ref="A1:AB602"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A254" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J8" sqref="J8"/>
+      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H275" sqref="H275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14678,7 +14678,7 @@
       </c>
       <c r="AB63" s="9">
         <f>'[1]Misc In_Out'!$C1160</f>
-        <v>287.60330578512395</v>
+        <v>297.52066115702479</v>
       </c>
     </row>
     <row r="64" spans="1:28" x14ac:dyDescent="0.25">
@@ -15128,7 +15128,7 @@
       </c>
       <c r="AB68" s="9">
         <f>'[1]Misc In_Out'!$C1165</f>
-        <v>156.099173553719</v>
+        <v>297.52066115702479</v>
       </c>
     </row>
     <row r="69" spans="1:28" x14ac:dyDescent="0.25">
@@ -15218,7 +15218,7 @@
       </c>
       <c r="AB69" s="9">
         <f>'[1]Misc In_Out'!$C1166</f>
-        <v>162.04958677685951</v>
+        <v>297.52066115702479</v>
       </c>
     </row>
     <row r="70" spans="1:28" x14ac:dyDescent="0.25">
@@ -15398,7 +15398,7 @@
       </c>
       <c r="AB71" s="9">
         <f>'[1]Misc In_Out'!$C1168</f>
-        <v>200.3305785123967</v>
+        <v>297.52066115702479</v>
       </c>
     </row>
     <row r="72" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>